<commit_message>
Modify Escenarios de pruebas con Gherking
</commit_message>
<xml_diff>
--- a/Repository-TestPlan/Documentation/Escenarios de prueba con Gherking.xlsx
+++ b/Repository-TestPlan/Documentation/Escenarios de prueba con Gherking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismael\Desktop\Repository-TestPlan\Repository-TestPlan\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD1FA28-B1E7-498B-8C52-FAD50F72508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E412D761-ED5B-4EA5-A082-A6A7BC0AD41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Identificador</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>PENDING</t>
+  </si>
+  <si>
+    <t>CP3</t>
   </si>
   <si>
     <t>CP1</t>
@@ -165,12 +168,21 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Confecciones de Jomar</t>
+  </si>
+  <si>
+    <t>REPORTE DE BUG</t>
+  </si>
+  <si>
+    <t>Registrar datos en la base de datos de manera correcta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -200,6 +212,20 @@
       <color theme="1"/>
       <name val="Poppins"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Poppins"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -221,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -258,17 +284,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dotted">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -298,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -319,12 +334,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -546,10 +567,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB995"/>
+  <dimension ref="A2:AB987"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -567,113 +588,22 @@
     <col min="11" max="16384" width="12.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-    </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
+      <c r="F2" s="11" t="s">
+        <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="273" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -693,34 +623,34 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="234" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
+      <c r="D4" s="4" t="s">
+        <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
+      <c r="F4" s="4" t="s">
+        <v>4</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
+      <c r="G4" s="4" t="s">
+        <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
+      <c r="H4" s="4" t="s">
+        <v>6</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>15</v>
+      <c r="I4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -741,17 +671,35 @@
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
     </row>
-    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="273" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="7"/>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -771,17 +719,35 @@
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="234" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -803,14 +769,14 @@
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -833,14 +799,14 @@
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -863,14 +829,16 @@
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -893,15 +861,33 @@
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="1"/>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -921,17 +907,21 @@
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="1"/>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -953,14 +943,14 @@
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -983,14 +973,14 @@
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1013,14 +1003,14 @@
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1041,7 +1031,7 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
     </row>
-    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1071,7 +1061,7 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1101,7 +1091,7 @@
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
     </row>
-    <row r="17" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1131,7 +1121,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1161,7 +1151,7 @@
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
     </row>
-    <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1191,7 +1181,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1221,7 +1211,7 @@
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1251,7 +1241,7 @@
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
     </row>
-    <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -30231,249 +30221,9 @@
       <c r="AA987" s="1"/>
       <c r="AB987" s="1"/>
     </row>
-    <row r="988" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A988" s="1"/>
-      <c r="B988" s="1"/>
-      <c r="C988" s="1"/>
-      <c r="D988" s="1"/>
-      <c r="E988" s="1"/>
-      <c r="F988" s="1"/>
-      <c r="G988" s="1"/>
-      <c r="H988" s="1"/>
-      <c r="I988" s="1"/>
-      <c r="J988" s="1"/>
-      <c r="K988" s="1"/>
-      <c r="L988" s="1"/>
-      <c r="M988" s="1"/>
-      <c r="N988" s="1"/>
-      <c r="O988" s="1"/>
-      <c r="P988" s="1"/>
-      <c r="Q988" s="1"/>
-      <c r="R988" s="1"/>
-      <c r="S988" s="1"/>
-      <c r="T988" s="1"/>
-      <c r="U988" s="1"/>
-      <c r="V988" s="1"/>
-      <c r="W988" s="1"/>
-      <c r="X988" s="1"/>
-      <c r="Y988" s="1"/>
-      <c r="Z988" s="1"/>
-      <c r="AA988" s="1"/>
-      <c r="AB988" s="1"/>
-    </row>
-    <row r="989" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A989" s="1"/>
-      <c r="B989" s="1"/>
-      <c r="C989" s="1"/>
-      <c r="D989" s="1"/>
-      <c r="E989" s="1"/>
-      <c r="F989" s="1"/>
-      <c r="G989" s="1"/>
-      <c r="H989" s="1"/>
-      <c r="I989" s="1"/>
-      <c r="J989" s="1"/>
-      <c r="K989" s="1"/>
-      <c r="L989" s="1"/>
-      <c r="M989" s="1"/>
-      <c r="N989" s="1"/>
-      <c r="O989" s="1"/>
-      <c r="P989" s="1"/>
-      <c r="Q989" s="1"/>
-      <c r="R989" s="1"/>
-      <c r="S989" s="1"/>
-      <c r="T989" s="1"/>
-      <c r="U989" s="1"/>
-      <c r="V989" s="1"/>
-      <c r="W989" s="1"/>
-      <c r="X989" s="1"/>
-      <c r="Y989" s="1"/>
-      <c r="Z989" s="1"/>
-      <c r="AA989" s="1"/>
-      <c r="AB989" s="1"/>
-    </row>
-    <row r="990" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A990" s="1"/>
-      <c r="B990" s="1"/>
-      <c r="C990" s="1"/>
-      <c r="D990" s="1"/>
-      <c r="E990" s="1"/>
-      <c r="F990" s="1"/>
-      <c r="G990" s="1"/>
-      <c r="H990" s="1"/>
-      <c r="I990" s="1"/>
-      <c r="J990" s="1"/>
-      <c r="K990" s="1"/>
-      <c r="L990" s="1"/>
-      <c r="M990" s="1"/>
-      <c r="N990" s="1"/>
-      <c r="O990" s="1"/>
-      <c r="P990" s="1"/>
-      <c r="Q990" s="1"/>
-      <c r="R990" s="1"/>
-      <c r="S990" s="1"/>
-      <c r="T990" s="1"/>
-      <c r="U990" s="1"/>
-      <c r="V990" s="1"/>
-      <c r="W990" s="1"/>
-      <c r="X990" s="1"/>
-      <c r="Y990" s="1"/>
-      <c r="Z990" s="1"/>
-      <c r="AA990" s="1"/>
-      <c r="AB990" s="1"/>
-    </row>
-    <row r="991" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A991" s="1"/>
-      <c r="B991" s="1"/>
-      <c r="C991" s="1"/>
-      <c r="D991" s="1"/>
-      <c r="E991" s="1"/>
-      <c r="F991" s="1"/>
-      <c r="G991" s="1"/>
-      <c r="H991" s="1"/>
-      <c r="I991" s="1"/>
-      <c r="J991" s="1"/>
-      <c r="K991" s="1"/>
-      <c r="L991" s="1"/>
-      <c r="M991" s="1"/>
-      <c r="N991" s="1"/>
-      <c r="O991" s="1"/>
-      <c r="P991" s="1"/>
-      <c r="Q991" s="1"/>
-      <c r="R991" s="1"/>
-      <c r="S991" s="1"/>
-      <c r="T991" s="1"/>
-      <c r="U991" s="1"/>
-      <c r="V991" s="1"/>
-      <c r="W991" s="1"/>
-      <c r="X991" s="1"/>
-      <c r="Y991" s="1"/>
-      <c r="Z991" s="1"/>
-      <c r="AA991" s="1"/>
-      <c r="AB991" s="1"/>
-    </row>
-    <row r="992" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A992" s="1"/>
-      <c r="B992" s="1"/>
-      <c r="C992" s="1"/>
-      <c r="D992" s="1"/>
-      <c r="E992" s="1"/>
-      <c r="F992" s="1"/>
-      <c r="G992" s="1"/>
-      <c r="H992" s="1"/>
-      <c r="I992" s="1"/>
-      <c r="J992" s="1"/>
-      <c r="K992" s="1"/>
-      <c r="L992" s="1"/>
-      <c r="M992" s="1"/>
-      <c r="N992" s="1"/>
-      <c r="O992" s="1"/>
-      <c r="P992" s="1"/>
-      <c r="Q992" s="1"/>
-      <c r="R992" s="1"/>
-      <c r="S992" s="1"/>
-      <c r="T992" s="1"/>
-      <c r="U992" s="1"/>
-      <c r="V992" s="1"/>
-      <c r="W992" s="1"/>
-      <c r="X992" s="1"/>
-      <c r="Y992" s="1"/>
-      <c r="Z992" s="1"/>
-      <c r="AA992" s="1"/>
-      <c r="AB992" s="1"/>
-    </row>
-    <row r="993" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A993" s="1"/>
-      <c r="B993" s="1"/>
-      <c r="C993" s="1"/>
-      <c r="D993" s="1"/>
-      <c r="E993" s="1"/>
-      <c r="F993" s="1"/>
-      <c r="G993" s="1"/>
-      <c r="H993" s="1"/>
-      <c r="I993" s="1"/>
-      <c r="J993" s="1"/>
-      <c r="K993" s="1"/>
-      <c r="L993" s="1"/>
-      <c r="M993" s="1"/>
-      <c r="N993" s="1"/>
-      <c r="O993" s="1"/>
-      <c r="P993" s="1"/>
-      <c r="Q993" s="1"/>
-      <c r="R993" s="1"/>
-      <c r="S993" s="1"/>
-      <c r="T993" s="1"/>
-      <c r="U993" s="1"/>
-      <c r="V993" s="1"/>
-      <c r="W993" s="1"/>
-      <c r="X993" s="1"/>
-      <c r="Y993" s="1"/>
-      <c r="Z993" s="1"/>
-      <c r="AA993" s="1"/>
-      <c r="AB993" s="1"/>
-    </row>
-    <row r="994" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A994" s="1"/>
-      <c r="B994" s="1"/>
-      <c r="C994" s="1"/>
-      <c r="D994" s="1"/>
-      <c r="E994" s="1"/>
-      <c r="F994" s="1"/>
-      <c r="G994" s="1"/>
-      <c r="H994" s="1"/>
-      <c r="I994" s="1"/>
-      <c r="J994" s="1"/>
-      <c r="K994" s="1"/>
-      <c r="L994" s="1"/>
-      <c r="M994" s="1"/>
-      <c r="N994" s="1"/>
-      <c r="O994" s="1"/>
-      <c r="P994" s="1"/>
-      <c r="Q994" s="1"/>
-      <c r="R994" s="1"/>
-      <c r="S994" s="1"/>
-      <c r="T994" s="1"/>
-      <c r="U994" s="1"/>
-      <c r="V994" s="1"/>
-      <c r="W994" s="1"/>
-      <c r="X994" s="1"/>
-      <c r="Y994" s="1"/>
-      <c r="Z994" s="1"/>
-      <c r="AA994" s="1"/>
-      <c r="AB994" s="1"/>
-    </row>
-    <row r="995" spans="1:28" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="A995" s="1"/>
-      <c r="B995" s="1"/>
-      <c r="C995" s="1"/>
-      <c r="D995" s="1"/>
-      <c r="E995" s="1"/>
-      <c r="F995" s="1"/>
-      <c r="G995" s="1"/>
-      <c r="H995" s="1"/>
-      <c r="I995" s="1"/>
-      <c r="J995" s="1"/>
-      <c r="K995" s="1"/>
-      <c r="L995" s="1"/>
-      <c r="M995" s="1"/>
-      <c r="N995" s="1"/>
-      <c r="O995" s="1"/>
-      <c r="P995" s="1"/>
-      <c r="Q995" s="1"/>
-      <c r="R995" s="1"/>
-      <c r="S995" s="1"/>
-      <c r="T995" s="1"/>
-      <c r="U995" s="1"/>
-      <c r="V995" s="1"/>
-      <c r="W995" s="1"/>
-      <c r="X995" s="1"/>
-      <c r="Y995" s="1"/>
-      <c r="Z995" s="1"/>
-      <c r="AA995" s="1"/>
-      <c r="AB995" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="I2:I995" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I4:I987" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PENDING,IN PROGRESS,BLOCKED,PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>